<commit_message>
Updated final SVM model
</commit_message>
<xml_diff>
--- a/results/SVM.xlsx
+++ b/results/SVM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="350">
   <si>
     <t>bestHyperparameters</t>
   </si>
@@ -1050,6 +1050,21 @@
   </si>
   <si>
     <t>{'shrinking': True, 'kernel': 'linear', 'gamma': 'auto', 'C': 1.83}</t>
+  </si>
+  <si>
+    <t>{'shrinking': True, 'kernel': 'linear', 'gamma': 'auto', 'degree': 3, 'C': 2.03}</t>
+  </si>
+  <si>
+    <t>{'shrinking': True, 'kernel': 'poly', 'gamma': 'scale', 'degree': 3, 'coef0': 7, 'C': 0.1}</t>
+  </si>
+  <si>
+    <t>{'C': 0.1, 'coef0': 7, 'degree': 3, 'gamma': 'scale', 'kernel': 'poly', 'shrinking': True}</t>
+  </si>
+  <si>
+    <t>{'C': 0.1, 'coef0': 6.99999999999994, 'degree': 3, 'gamma': 'scale', 'kernel': 'poly', 'shrinking': True}</t>
+  </si>
+  <si>
+    <t>{'C': 0.1, 'coef0': 7.0, 'degree': 3, 'gamma': 'scale', 'kernel': 'poly', 'shrinking': True}</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C366"/>
+  <dimension ref="A1:C372"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A148" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C320" activeCellId="0" pane="topLeft" sqref="A164:C320"/>
@@ -5473,6 +5488,72 @@
         <v>0.783</v>
       </c>
     </row>
+    <row r="367" spans="1:3">
+      <c r="A367" t="s">
+        <v>345</v>
+      </c>
+      <c r="B367" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="C367" t="n">
+        <v>0.767</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3">
+      <c r="A368" t="s">
+        <v>346</v>
+      </c>
+      <c r="B368" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C368" t="n">
+        <v>0.767</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3">
+      <c r="A369" t="s">
+        <v>347</v>
+      </c>
+      <c r="B369" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C369" t="n">
+        <v>0.767</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3">
+      <c r="A370" t="s">
+        <v>348</v>
+      </c>
+      <c r="B370" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C370" t="n">
+        <v>0.767</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3">
+      <c r="A371" t="s">
+        <v>349</v>
+      </c>
+      <c r="B371" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C371" t="n">
+        <v>0.767</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3">
+      <c r="A372" t="s">
+        <v>349</v>
+      </c>
+      <c r="B372" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C372" t="n">
+        <v>0.767</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>

</xml_diff>